<commit_message>
All three whisper models integrated
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -414,7 +414,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -454,7 +454,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the dataset for the metrics calculation
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -414,7 +414,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -446,7 +446,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2">

</xml_diff>